<commit_message>
cfg1 PIN12 for l12
</commit_message>
<xml_diff>
--- a/doc/clock_1060M.xlsx
+++ b/doc/clock_1060M.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cxwao\Documents\GitHub2\GreenPAK_7seg\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDC9183-81DD-4B58-84FA-58E953E63F67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7966745F-74EC-4AC5-A4E0-BA1500256D49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16260" yWindow="1410" windowWidth="19065" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="345" windowWidth="12090" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TDCG1060M" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="186">
   <si>
     <t>VDD</t>
     <phoneticPr fontId="2"/>
@@ -96,10 +96,6 @@
   </si>
   <si>
     <t>CLK</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>dp</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -616,10 +612,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>PullUp</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Common Cathode</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -656,10 +648,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>--</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>VDD1</t>
   </si>
   <si>
@@ -708,9 +696,6 @@
     <t>B3,B24</t>
   </si>
   <si>
-    <t>I,PU10k</t>
-  </si>
-  <si>
     <t>IO1</t>
   </si>
   <si>
@@ -748,6 +733,26 @@
   </si>
   <si>
     <t>dig4</t>
+  </si>
+  <si>
+    <t>l12</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>32768Hz RTC</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>VDD1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>VDD2</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -1197,6 +1202,69 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
@@ -1214,69 +1282,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1796,8 +1801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AA60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1818,59 +1823,62 @@
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B2" s="44" t="s">
-        <v>134</v>
+        <v>133</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B4" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F4" s="44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B6" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="F6" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="D6" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="17" t="s">
+      <c r="I6" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="L6" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="L6" s="17" t="s">
-        <v>126</v>
-      </c>
       <c r="M6" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B7" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C7" s="53" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="55"/>
       <c r="E7" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
@@ -1884,24 +1892,24 @@
         <v>1</v>
       </c>
       <c r="K7" s="46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L7" s="46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B8" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="31" t="s">
-        <v>47</v>
-      </c>
       <c r="D8" s="47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>2</v>
@@ -1918,24 +1926,24 @@
         <v>3</v>
       </c>
       <c r="K8" s="47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L8" s="47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B9" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>4</v>
@@ -1952,24 +1960,24 @@
         <v>5</v>
       </c>
       <c r="K9" s="47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L9" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B10" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>6</v>
@@ -1986,24 +1994,24 @@
         <v>7</v>
       </c>
       <c r="K10" s="47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L10" s="47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B11" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>9</v>
@@ -2020,24 +2028,24 @@
         <v>10</v>
       </c>
       <c r="K11" s="51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L11" s="48" t="s">
         <v>20</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B12" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>11</v>
@@ -2054,24 +2062,24 @@
         <v>12</v>
       </c>
       <c r="K12" s="47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L12" s="47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B13" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>13</v>
@@ -2089,7 +2097,7 @@
       </c>
       <c r="K13" s="49"/>
       <c r="L13" s="49" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M13" s="17" t="s">
         <v>14</v>
@@ -2097,13 +2105,13 @@
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B14" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D14" s="47" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>15</v>
@@ -2120,24 +2128,24 @@
         <v>16</v>
       </c>
       <c r="K14" s="47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L14" s="47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M14" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B15" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D15" s="47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>17</v>
@@ -2154,24 +2162,24 @@
         <v>18</v>
       </c>
       <c r="K15" s="57" t="s">
-        <v>154</v>
+        <v>54</v>
       </c>
       <c r="L15" s="57" t="s">
-        <v>154</v>
+        <v>181</v>
       </c>
       <c r="M15" s="17" t="s">
-        <v>45</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B16" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C16" s="54" t="s">
-        <v>21</v>
+        <v>132</v>
       </c>
       <c r="D16" s="52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>19</v>
@@ -2192,76 +2200,76 @@
         <v>8</v>
       </c>
       <c r="M16" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B19" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F19" s="44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="Q20" s="64"/>
-      <c r="R20" s="64"/>
-      <c r="S20" s="64"/>
-      <c r="T20" s="64"/>
-      <c r="U20" s="64"/>
-      <c r="V20" s="64"/>
+      <c r="Q20" s="58"/>
+      <c r="R20" s="58"/>
+      <c r="S20" s="58"/>
+      <c r="T20" s="58"/>
+      <c r="U20" s="58"/>
+      <c r="V20" s="58"/>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B21" s="71" t="s">
+      <c r="B21" s="65" t="s">
+        <v>123</v>
+      </c>
+      <c r="C21" s="65" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="E21" s="65" t="s">
         <v>124</v>
       </c>
-      <c r="C21" s="71" t="s">
+      <c r="F21" s="16" t="s">
         <v>126</v>
-      </c>
-      <c r="D21" s="71" t="s">
-        <v>132</v>
-      </c>
-      <c r="E21" s="71" t="s">
-        <v>125</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>127</v>
       </c>
       <c r="G21" s="21"/>
       <c r="H21" s="21"/>
       <c r="I21" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J21" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="K21" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="L21" s="65" t="s">
         <v>125</v>
       </c>
-      <c r="K21" s="71" t="s">
-        <v>132</v>
-      </c>
-      <c r="L21" s="71" t="s">
-        <v>126</v>
-      </c>
-      <c r="M21" s="71" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q21" s="64"/>
-      <c r="R21" s="64"/>
-      <c r="S21" s="64"/>
-      <c r="T21" s="64"/>
-      <c r="U21" s="64"/>
-      <c r="V21" s="64"/>
-      <c r="AA21" s="64"/>
+      <c r="M21" s="65" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q21" s="58"/>
+      <c r="R21" s="58"/>
+      <c r="S21" s="58"/>
+      <c r="T21" s="58"/>
+      <c r="U21" s="58"/>
+      <c r="V21" s="58"/>
+      <c r="AA21" s="58"/>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B22" s="72" t="s">
-        <v>155</v>
-      </c>
-      <c r="C22" s="84" t="s">
-        <v>166</v>
-      </c>
-      <c r="D22" s="83"/>
-      <c r="E22" s="67" t="s">
-        <v>166</v>
+      <c r="B22" s="66" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" s="78" t="s">
+        <v>163</v>
+      </c>
+      <c r="D22" s="77"/>
+      <c r="E22" s="61" t="s">
+        <v>184</v>
       </c>
       <c r="F22" s="6">
         <v>1</v>
@@ -2274,35 +2282,35 @@
       <c r="J22" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="K22" s="77" t="s">
+      <c r="K22" s="71" t="s">
+        <v>162</v>
+      </c>
+      <c r="L22" s="59" t="s">
+        <v>161</v>
+      </c>
+      <c r="M22" s="66" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q22" s="58"/>
+      <c r="R22" s="58"/>
+      <c r="S22" s="58"/>
+      <c r="T22" s="58"/>
+      <c r="U22" s="58"/>
+      <c r="V22" s="58"/>
+      <c r="AA22" s="58"/>
+    </row>
+    <row r="23" spans="2:27" x14ac:dyDescent="0.15">
+      <c r="B23" s="66" t="s">
+        <v>167</v>
+      </c>
+      <c r="C23" s="67" t="s">
+        <v>166</v>
+      </c>
+      <c r="D23" s="71" t="s">
+        <v>162</v>
+      </c>
+      <c r="E23" s="60" t="s">
         <v>165</v>
-      </c>
-      <c r="L22" s="65" t="s">
-        <v>164</v>
-      </c>
-      <c r="M22" s="72" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q22" s="64"/>
-      <c r="R22" s="64"/>
-      <c r="S22" s="64"/>
-      <c r="T22" s="64"/>
-      <c r="U22" s="64"/>
-      <c r="V22" s="64"/>
-      <c r="AA22" s="64"/>
-    </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B23" s="72" t="s">
-        <v>170</v>
-      </c>
-      <c r="C23" s="73" t="s">
-        <v>169</v>
-      </c>
-      <c r="D23" s="77" t="s">
-        <v>165</v>
-      </c>
-      <c r="E23" s="66" t="s">
-        <v>168</v>
       </c>
       <c r="F23" s="6">
         <v>2</v>
@@ -2315,35 +2323,35 @@
       <c r="J23" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K23" s="77" t="s">
-        <v>165</v>
-      </c>
-      <c r="L23" s="65" t="s">
-        <v>167</v>
-      </c>
-      <c r="M23" s="72" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q23" s="64"/>
-      <c r="R23" s="64"/>
-      <c r="S23" s="64"/>
-      <c r="T23" s="64"/>
-      <c r="U23" s="64"/>
-      <c r="V23" s="64"/>
-      <c r="AA23" s="64"/>
+      <c r="K23" s="71" t="s">
+        <v>162</v>
+      </c>
+      <c r="L23" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="M23" s="66" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q23" s="58"/>
+      <c r="R23" s="58"/>
+      <c r="S23" s="58"/>
+      <c r="T23" s="58"/>
+      <c r="U23" s="58"/>
+      <c r="V23" s="58"/>
+      <c r="AA23" s="58"/>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B24" s="67" t="s">
-        <v>174</v>
-      </c>
-      <c r="C24" s="73" t="s">
-        <v>174</v>
-      </c>
-      <c r="D24" s="77" t="s">
-        <v>173</v>
-      </c>
-      <c r="E24" s="67" t="s">
-        <v>172</v>
+      <c r="B24" s="61" t="s">
+        <v>170</v>
+      </c>
+      <c r="C24" s="67" t="s">
+        <v>170</v>
+      </c>
+      <c r="D24" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="E24" s="61" t="s">
+        <v>168</v>
       </c>
       <c r="F24" s="6">
         <v>3</v>
@@ -2356,34 +2364,34 @@
       <c r="J24" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K24" s="77" t="s">
+      <c r="K24" s="71" t="s">
+        <v>182</v>
+      </c>
+      <c r="L24" s="59" t="s">
+        <v>155</v>
+      </c>
+      <c r="M24" s="66" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q24" s="58"/>
+      <c r="R24" s="58"/>
+      <c r="S24" s="58"/>
+      <c r="T24" s="58"/>
+      <c r="U24" s="58"/>
+      <c r="V24" s="58"/>
+      <c r="AA24" s="58"/>
+    </row>
+    <row r="25" spans="2:27" x14ac:dyDescent="0.15">
+      <c r="B25" s="61" t="s">
         <v>171</v>
       </c>
-      <c r="L24" s="65" t="s">
-        <v>158</v>
-      </c>
-      <c r="M24" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q24" s="64"/>
-      <c r="R24" s="64"/>
-      <c r="S24" s="64"/>
-      <c r="T24" s="64"/>
-      <c r="U24" s="64"/>
-      <c r="V24" s="64"/>
-      <c r="AA24" s="64"/>
-    </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B25" s="67" t="s">
-        <v>175</v>
-      </c>
-      <c r="C25" s="73" t="s">
-        <v>175</v>
-      </c>
-      <c r="D25" s="81" t="s">
-        <v>173</v>
-      </c>
-      <c r="E25" s="66" t="s">
+      <c r="C25" s="67" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25" s="75" t="s">
+        <v>169</v>
+      </c>
+      <c r="E25" s="60" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="6">
@@ -2397,34 +2405,34 @@
       <c r="J25" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K25" s="77" t="s">
-        <v>173</v>
-      </c>
-      <c r="L25" s="65" t="s">
-        <v>159</v>
-      </c>
-      <c r="M25" s="67" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q25" s="64"/>
-      <c r="R25" s="64"/>
-      <c r="S25" s="64"/>
-      <c r="T25" s="64"/>
-      <c r="U25" s="64"/>
-      <c r="V25" s="64"/>
-      <c r="AA25" s="64"/>
+      <c r="K25" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="L25" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="M25" s="61" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q25" s="58"/>
+      <c r="R25" s="58"/>
+      <c r="S25" s="58"/>
+      <c r="T25" s="58"/>
+      <c r="U25" s="58"/>
+      <c r="V25" s="58"/>
+      <c r="AA25" s="58"/>
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B26" s="67" t="s">
-        <v>176</v>
-      </c>
-      <c r="C26" s="73" t="s">
-        <v>176</v>
-      </c>
-      <c r="D26" s="82" t="s">
-        <v>173</v>
-      </c>
-      <c r="E26" s="66" t="s">
+      <c r="B26" s="61" t="s">
+        <v>172</v>
+      </c>
+      <c r="C26" s="67" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="E26" s="60" t="s">
         <v>9</v>
       </c>
       <c r="F26" s="6">
@@ -2438,34 +2446,34 @@
       <c r="J26" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K26" s="77" t="s">
+      <c r="K26" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="L26" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="M26" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q26" s="58"/>
+      <c r="R26" s="58"/>
+      <c r="S26" s="58"/>
+      <c r="T26" s="58"/>
+      <c r="U26" s="58"/>
+      <c r="V26" s="58"/>
+      <c r="AA26" s="58"/>
+    </row>
+    <row r="27" spans="2:27" x14ac:dyDescent="0.15">
+      <c r="B27" s="61" t="s">
         <v>173</v>
       </c>
-      <c r="L26" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="M26" s="67" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q26" s="64"/>
-      <c r="R26" s="64"/>
-      <c r="S26" s="64"/>
-      <c r="T26" s="64"/>
-      <c r="U26" s="64"/>
-      <c r="V26" s="64"/>
-      <c r="AA26" s="64"/>
-    </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B27" s="67" t="s">
-        <v>177</v>
-      </c>
-      <c r="C27" s="73" t="s">
-        <v>177</v>
-      </c>
-      <c r="D27" s="77" t="s">
+      <c r="C27" s="67" t="s">
         <v>173</v>
       </c>
-      <c r="E27" s="68" t="s">
+      <c r="D27" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="E27" s="62" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="6">
@@ -2479,34 +2487,34 @@
       <c r="J27" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K27" s="77" t="s">
-        <v>173</v>
-      </c>
-      <c r="L27" s="65" t="s">
-        <v>160</v>
-      </c>
-      <c r="M27" s="67" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q27" s="64"/>
-      <c r="R27" s="64"/>
-      <c r="S27" s="64"/>
-      <c r="T27" s="64"/>
-      <c r="U27" s="64"/>
-      <c r="V27" s="64"/>
-      <c r="AA27" s="64"/>
+      <c r="K27" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="L27" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="M27" s="61" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q27" s="58"/>
+      <c r="R27" s="58"/>
+      <c r="S27" s="58"/>
+      <c r="T27" s="58"/>
+      <c r="U27" s="58"/>
+      <c r="V27" s="58"/>
+      <c r="AA27" s="58"/>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B28" s="67" t="s">
-        <v>178</v>
-      </c>
-      <c r="C28" s="73" t="s">
-        <v>178</v>
-      </c>
-      <c r="D28" s="77" t="s">
-        <v>173</v>
-      </c>
-      <c r="E28" s="68" t="s">
+      <c r="B28" s="61" t="s">
+        <v>174</v>
+      </c>
+      <c r="C28" s="67" t="s">
+        <v>174</v>
+      </c>
+      <c r="D28" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="E28" s="62" t="s">
         <v>13</v>
       </c>
       <c r="F28" s="7">
@@ -2520,33 +2528,33 @@
       <c r="J28" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K28" s="78"/>
-      <c r="L28" s="74" t="s">
-        <v>166</v>
-      </c>
-      <c r="M28" s="72" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q28" s="64"/>
-      <c r="R28" s="64"/>
-      <c r="S28" s="64"/>
-      <c r="T28" s="64"/>
-      <c r="U28" s="64"/>
-      <c r="V28" s="64"/>
-      <c r="AA28" s="64"/>
+      <c r="K28" s="72"/>
+      <c r="L28" s="68" t="s">
+        <v>163</v>
+      </c>
+      <c r="M28" s="66" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q28" s="58"/>
+      <c r="R28" s="58"/>
+      <c r="S28" s="58"/>
+      <c r="T28" s="58"/>
+      <c r="U28" s="58"/>
+      <c r="V28" s="58"/>
+      <c r="AA28" s="58"/>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B29" s="72" t="s">
-        <v>179</v>
-      </c>
-      <c r="C29" s="73" t="s">
-        <v>179</v>
-      </c>
-      <c r="D29" s="77" t="s">
-        <v>180</v>
-      </c>
-      <c r="E29" s="69" t="s">
-        <v>179</v>
+      <c r="B29" s="66" t="s">
+        <v>175</v>
+      </c>
+      <c r="C29" s="67" t="s">
+        <v>175</v>
+      </c>
+      <c r="D29" s="71" t="s">
+        <v>176</v>
+      </c>
+      <c r="E29" s="63" t="s">
+        <v>175</v>
       </c>
       <c r="F29" s="7">
         <v>8</v>
@@ -2559,35 +2567,35 @@
       <c r="J29" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K29" s="77" t="s">
-        <v>173</v>
-      </c>
-      <c r="L29" s="65" t="s">
-        <v>161</v>
-      </c>
-      <c r="M29" s="67" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q29" s="64"/>
-      <c r="R29" s="64"/>
-      <c r="S29" s="64"/>
-      <c r="T29" s="64"/>
-      <c r="U29" s="64"/>
-      <c r="V29" s="64"/>
-      <c r="AA29" s="64"/>
+      <c r="K29" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="L29" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="M29" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q29" s="58"/>
+      <c r="R29" s="58"/>
+      <c r="S29" s="58"/>
+      <c r="T29" s="58"/>
+      <c r="U29" s="58"/>
+      <c r="V29" s="58"/>
+      <c r="AA29" s="58"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B30" s="72" t="s">
-        <v>181</v>
-      </c>
-      <c r="C30" s="73" t="s">
-        <v>181</v>
-      </c>
-      <c r="D30" s="77" t="s">
-        <v>182</v>
-      </c>
-      <c r="E30" s="69" t="s">
-        <v>181</v>
+      <c r="B30" s="66" t="s">
+        <v>177</v>
+      </c>
+      <c r="C30" s="67" t="s">
+        <v>177</v>
+      </c>
+      <c r="D30" s="71" t="s">
+        <v>178</v>
+      </c>
+      <c r="E30" s="63" t="s">
+        <v>177</v>
       </c>
       <c r="F30" s="7">
         <v>9</v>
@@ -2600,35 +2608,35 @@
       <c r="J30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="K30" s="77" t="s">
-        <v>173</v>
-      </c>
-      <c r="L30" s="65" t="s">
-        <v>162</v>
-      </c>
-      <c r="M30" s="67" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q30" s="64"/>
-      <c r="R30" s="64"/>
-      <c r="S30" s="64"/>
-      <c r="T30" s="64"/>
-      <c r="U30" s="64"/>
-      <c r="V30" s="64"/>
-      <c r="AA30" s="67"/>
+      <c r="K30" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="L30" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="M30" s="61" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q30" s="58"/>
+      <c r="R30" s="58"/>
+      <c r="S30" s="58"/>
+      <c r="T30" s="58"/>
+      <c r="U30" s="58"/>
+      <c r="V30" s="58"/>
+      <c r="AA30" s="61"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B31" s="67" t="s">
-        <v>184</v>
-      </c>
-      <c r="C31" s="76" t="s">
-        <v>184</v>
-      </c>
-      <c r="D31" s="80" t="s">
-        <v>173</v>
-      </c>
-      <c r="E31" s="70" t="s">
-        <v>183</v>
+      <c r="B31" s="61" t="s">
+        <v>180</v>
+      </c>
+      <c r="C31" s="70" t="s">
+        <v>180</v>
+      </c>
+      <c r="D31" s="74" t="s">
+        <v>169</v>
+      </c>
+      <c r="E31" s="64" t="s">
+        <v>179</v>
       </c>
       <c r="F31" s="14">
         <v>10</v>
@@ -2641,29 +2649,29 @@
       <c r="J31" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="K31" s="79"/>
-      <c r="L31" s="75" t="s">
-        <v>163</v>
-      </c>
-      <c r="M31" s="72" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q31" s="64"/>
-      <c r="R31" s="64"/>
-      <c r="S31" s="64"/>
-      <c r="T31" s="64"/>
-      <c r="U31" s="64"/>
-      <c r="V31" s="64"/>
-      <c r="AA31" s="64"/>
+      <c r="K31" s="73"/>
+      <c r="L31" s="69" t="s">
+        <v>160</v>
+      </c>
+      <c r="M31" s="66" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q31" s="58"/>
+      <c r="R31" s="58"/>
+      <c r="S31" s="58"/>
+      <c r="T31" s="58"/>
+      <c r="U31" s="58"/>
+      <c r="V31" s="58"/>
+      <c r="AA31" s="58"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.15">
       <c r="E32"/>
-      <c r="Q32" s="64"/>
-      <c r="R32" s="64"/>
-      <c r="S32" s="64"/>
-      <c r="T32" s="64"/>
-      <c r="U32" s="64"/>
-      <c r="V32" s="64"/>
+      <c r="Q32" s="58"/>
+      <c r="R32" s="58"/>
+      <c r="S32" s="58"/>
+      <c r="T32" s="58"/>
+      <c r="U32" s="58"/>
+      <c r="V32" s="58"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B34" s="38"/>
@@ -2684,11 +2692,11 @@
     <row r="35" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B35" s="37"/>
       <c r="C35" s="41" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D35" s="42"/>
       <c r="E35" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K35" s="42"/>
       <c r="L35" s="8"/>
@@ -2711,18 +2719,18 @@
       <c r="C37" s="41"/>
       <c r="D37" s="42"/>
       <c r="E37" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
       <c r="I37" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J37" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K37" s="42"/>
       <c r="L37" s="8"/>
@@ -2736,10 +2744,10 @@
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="9"/>
-      <c r="G38" s="62">
+      <c r="G38" s="83">
         <v>8</v>
       </c>
-      <c r="H38" s="63"/>
+      <c r="H38" s="84"/>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
       <c r="K38" s="8"/>
@@ -2753,18 +2761,18 @@
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F39" s="8">
         <v>1</v>
       </c>
-      <c r="G39" s="58"/>
-      <c r="H39" s="59"/>
+      <c r="G39" s="79"/>
+      <c r="H39" s="80"/>
       <c r="I39" s="45">
         <v>16</v>
       </c>
       <c r="J39" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
@@ -2777,20 +2785,20 @@
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F40" s="8">
         <v>2</v>
       </c>
-      <c r="G40" s="58">
+      <c r="G40" s="79">
         <v>8</v>
       </c>
-      <c r="H40" s="59"/>
+      <c r="H40" s="80"/>
       <c r="I40" s="45">
         <v>15</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
@@ -2803,18 +2811,18 @@
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F41" s="8">
         <v>3</v>
       </c>
-      <c r="G41" s="58"/>
-      <c r="H41" s="59"/>
+      <c r="G41" s="79"/>
+      <c r="H41" s="80"/>
       <c r="I41" s="45">
         <v>14</v>
       </c>
       <c r="J41" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K41" s="8"/>
       <c r="L41" s="8"/>
@@ -2827,20 +2835,20 @@
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F42" s="8">
         <v>4</v>
       </c>
-      <c r="G42" s="58" t="s">
-        <v>38</v>
-      </c>
-      <c r="H42" s="59"/>
+      <c r="G42" s="79" t="s">
+        <v>37</v>
+      </c>
+      <c r="H42" s="80"/>
       <c r="I42" s="45">
         <v>13</v>
       </c>
       <c r="J42" s="45" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
@@ -2853,20 +2861,20 @@
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F43" s="8">
         <v>5</v>
       </c>
-      <c r="G43" s="58">
+      <c r="G43" s="79">
         <v>8</v>
       </c>
-      <c r="H43" s="59"/>
+      <c r="H43" s="80"/>
       <c r="I43" s="45">
         <v>12</v>
       </c>
       <c r="J43" s="45" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
@@ -2879,18 +2887,18 @@
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F44" s="8">
         <v>6</v>
       </c>
-      <c r="G44" s="58"/>
-      <c r="H44" s="59"/>
+      <c r="G44" s="79"/>
+      <c r="H44" s="80"/>
       <c r="I44" s="45">
         <v>11</v>
       </c>
       <c r="J44" s="45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
@@ -2906,10 +2914,10 @@
       <c r="F45" s="10">
         <v>7</v>
       </c>
-      <c r="G45" s="58">
+      <c r="G45" s="79">
         <v>8</v>
       </c>
-      <c r="H45" s="59"/>
+      <c r="H45" s="80"/>
       <c r="I45" s="45">
         <v>10</v>
       </c>
@@ -2925,13 +2933,13 @@
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F46" s="10">
         <v>8</v>
       </c>
-      <c r="G46" s="60"/>
-      <c r="H46" s="61"/>
+      <c r="G46" s="81"/>
+      <c r="H46" s="82"/>
       <c r="I46" s="45">
         <v>9</v>
       </c>
@@ -3188,8 +3196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:AE63"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AD45" sqref="AD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3213,73 +3221,73 @@
   <sheetData>
     <row r="2" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="X2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AC2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="2:31" x14ac:dyDescent="0.15">
       <c r="R3" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="S3" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="S3" s="17" t="s">
+      <c r="T3" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="T3" s="17" t="s">
+      <c r="U3" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="U3" s="17" t="s">
-        <v>76</v>
       </c>
       <c r="W3" s="27"/>
       <c r="X3" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y3" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z3" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AB3" s="27"/>
       <c r="AC3" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD3" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AE3" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="2:31" x14ac:dyDescent="0.15">
       <c r="H4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" t="s">
         <v>65</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>66</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>67</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>68</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>69</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>70</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>71</v>
-      </c>
-      <c r="O4" t="s">
-        <v>72</v>
       </c>
       <c r="R4" s="17">
         <v>8</v>
@@ -3294,28 +3302,28 @@
         <v>1</v>
       </c>
       <c r="W4" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="X4" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Y4" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Z4" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AB4" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC4" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AD4" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE4" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="2:31" ht="5.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3386,24 +3394,24 @@
         <v>0</v>
       </c>
       <c r="W6" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="X6" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Y6" s="23"/>
       <c r="Z6" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AB6" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC6" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AD6" s="23"/>
       <c r="AE6" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="2:31" ht="4.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3425,24 +3433,24 @@
         <v>1</v>
       </c>
       <c r="W8" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X8" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Y8" s="23"/>
       <c r="Z8" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AB8" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AC8" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AD8" s="23"/>
       <c r="AE8" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="2:31" ht="5.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3461,28 +3469,28 @@
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.15">
       <c r="W10" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="X10" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Y10" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z10" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AB10" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AC10" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AD10" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AE10" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="2:31" ht="5.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3549,24 +3557,24 @@
         <v>1</v>
       </c>
       <c r="W12" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X12" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Y12" s="23"/>
       <c r="Z12" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AB12" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC12" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AD12" s="23"/>
       <c r="AE12" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="2:31" ht="4.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3586,28 +3594,28 @@
         <v>1</v>
       </c>
       <c r="W14" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X14" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Y14" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Z14" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AB14" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AC14" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AD14" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AE14" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="2:31" ht="5.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3624,28 +3632,28 @@
     </row>
     <row r="16" spans="2:31" x14ac:dyDescent="0.15">
       <c r="W16" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="X16" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Y16" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Z16" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AB16" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AC16" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AD16" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AE16" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="2:31" ht="5.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3714,24 +3722,24 @@
         <v>0</v>
       </c>
       <c r="W18" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="X18" s="9"/>
       <c r="Y18" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Z18" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AB18" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AC18" s="9"/>
       <c r="AD18" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AE18" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="2:31" ht="4.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3753,24 +3761,24 @@
       </c>
       <c r="E20" s="19"/>
       <c r="W20" s="29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="X20" s="9"/>
       <c r="Y20" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Z20" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AB20" s="29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AC20" s="9"/>
       <c r="AD20" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AE20" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="2:31" ht="5.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3789,24 +3797,24 @@
     </row>
     <row r="22" spans="2:31" x14ac:dyDescent="0.15">
       <c r="W22" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="X22" s="9"/>
       <c r="Y22" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Z22" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AB22" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AC22" s="9"/>
       <c r="AD22" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AE22" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="2:31" ht="5.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3875,24 +3883,24 @@
         <v>1</v>
       </c>
       <c r="W24" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X24" s="9"/>
       <c r="Y24" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Z24" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AB24" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AC24" s="9"/>
       <c r="AD24" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AE24" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="2:31" ht="4.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3915,10 +3923,10 @@
       </c>
       <c r="W26" s="38"/>
       <c r="X26" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Y26" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Z26" s="28">
         <v>4</v>
@@ -3926,10 +3934,10 @@
       <c r="AA26" s="9"/>
       <c r="AB26" s="38"/>
       <c r="AC26" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AD26" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AE26" s="28">
         <v>4</v>
@@ -3954,7 +3962,7 @@
       <c r="W28" s="35"/>
       <c r="X28" s="21"/>
       <c r="Y28" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Z28" s="30">
         <v>7</v>
@@ -3963,7 +3971,7 @@
       <c r="AB28" s="35"/>
       <c r="AC28" s="21"/>
       <c r="AD28" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AE28" s="30">
         <v>7</v>
@@ -4027,7 +4035,7 @@
         <v>0</v>
       </c>
       <c r="AC30" s="41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="2:31" ht="4.5" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
cfg1 PIN12,16 and OSC1 removed
</commit_message>
<xml_diff>
--- a/doc/clock_1060M.xlsx
+++ b/doc/clock_1060M.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cxwao\Documents\GitHub2\GreenPAK_7seg\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7966745F-74EC-4AC5-A4E0-BA1500256D49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF791EC-71E3-41FE-876A-55F53435F43F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="345" windowWidth="12090" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="4170" windowWidth="12090" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TDCG1060M" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="184">
   <si>
     <t>VDD</t>
     <phoneticPr fontId="2"/>
@@ -95,10 +95,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>CLK</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>A24</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -243,10 +239,6 @@
   </si>
   <si>
     <t>SDA</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>IO,PU10k</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -569,10 +561,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>digC</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>24H version</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -636,10 +624,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>#digC</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>#deg4</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -752,6 +736,14 @@
   </si>
   <si>
     <t>VDD2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>-</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -759,7 +751,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -795,14 +787,6 @@
       <color rgb="FFFF0000"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -1082,7 +1066,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
@@ -1121,9 +1105,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1151,7 +1132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1196,7 +1177,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1256,7 +1237,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1265,23 +1246,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1801,8 +1785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AA60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1822,63 +1806,63 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B2" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="D2" s="44" t="s">
-        <v>183</v>
+      <c r="B2" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B4" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="F4" s="44" t="s">
-        <v>134</v>
+        <v>142</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B6" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>125</v>
-      </c>
       <c r="D6" s="17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E6" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>126</v>
-      </c>
       <c r="I6" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B7" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="55"/>
+        <v>102</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="54"/>
       <c r="E7" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
@@ -1891,25 +1875,25 @@
       <c r="J7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="L7" s="46" t="s">
-        <v>25</v>
+      <c r="K7" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7" s="45" t="s">
+        <v>24</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B8" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="47" t="s">
-        <v>59</v>
+      <c r="D8" s="46" t="s">
+        <v>57</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>2</v>
@@ -1925,25 +1909,25 @@
       <c r="J8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="L8" s="47" t="s">
-        <v>26</v>
+      <c r="K8" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="46" t="s">
+        <v>25</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B9" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="51" t="s">
-        <v>63</v>
+        <v>37</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>61</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>4</v>
@@ -1959,25 +1943,25 @@
       <c r="J9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K9" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="L9" s="47" t="s">
-        <v>24</v>
+      <c r="K9" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9" s="46" t="s">
+        <v>23</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B10" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="56" t="s">
-        <v>61</v>
+        <v>38</v>
+      </c>
+      <c r="D10" s="55" t="s">
+        <v>59</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>6</v>
@@ -1993,25 +1977,25 @@
       <c r="J10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="L10" s="47" t="s">
-        <v>27</v>
+      <c r="K10" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="L10" s="46" t="s">
+        <v>26</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B11" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="56" t="s">
-        <v>61</v>
+        <v>39</v>
+      </c>
+      <c r="D11" s="55" t="s">
+        <v>59</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>9</v>
@@ -2027,25 +2011,25 @@
       <c r="J11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="L11" s="48" t="s">
-        <v>20</v>
+      <c r="K11" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="L11" s="47" t="s">
+        <v>182</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B12" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="47" t="s">
-        <v>55</v>
+        <v>21</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>54</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>11</v>
@@ -2061,25 +2045,25 @@
       <c r="J12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="L12" s="47" t="s">
-        <v>21</v>
+      <c r="K12" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L12" s="46" t="s">
+        <v>20</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B13" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="51" t="s">
-        <v>55</v>
+        <v>22</v>
+      </c>
+      <c r="D13" s="50" t="s">
+        <v>54</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>13</v>
@@ -2095,9 +2079,9 @@
       <c r="J13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K13" s="49"/>
-      <c r="L13" s="49" t="s">
-        <v>103</v>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48" t="s">
+        <v>101</v>
       </c>
       <c r="M13" s="17" t="s">
         <v>14</v>
@@ -2105,13 +2089,13 @@
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B14" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D14" s="47" t="s">
         <v>127</v>
+      </c>
+      <c r="D14" s="46" t="s">
+        <v>125</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>15</v>
@@ -2127,25 +2111,25 @@
       <c r="J14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K14" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="L14" s="47" t="s">
-        <v>99</v>
+      <c r="K14" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="L14" s="46" t="s">
+        <v>97</v>
       </c>
       <c r="M14" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B15" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D15" s="47" t="s">
         <v>128</v>
+      </c>
+      <c r="D15" s="46" t="s">
+        <v>126</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>17</v>
@@ -2161,25 +2145,25 @@
       <c r="J15" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="L15" s="57" t="s">
-        <v>181</v>
+      <c r="K15" s="56" t="s">
+        <v>183</v>
+      </c>
+      <c r="L15" s="56" t="s">
+        <v>183</v>
       </c>
       <c r="M15" s="17" t="s">
-        <v>181</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B16" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="C16" s="54" t="s">
-        <v>132</v>
-      </c>
-      <c r="D16" s="52" t="s">
-        <v>54</v>
+        <v>177</v>
+      </c>
+      <c r="C16" s="53" t="s">
+        <v>177</v>
+      </c>
+      <c r="D16" s="51" t="s">
+        <v>53</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>19</v>
@@ -2195,81 +2179,81 @@
       <c r="J16" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="K16" s="50"/>
-      <c r="L16" s="50" t="s">
+      <c r="K16" s="49"/>
+      <c r="L16" s="49" t="s">
         <v>8</v>
       </c>
       <c r="M16" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B19" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="F19" s="44" t="s">
-        <v>134</v>
+        <v>143</v>
+      </c>
+      <c r="F19" s="43" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="Q20" s="58"/>
-      <c r="R20" s="58"/>
-      <c r="S20" s="58"/>
-      <c r="T20" s="58"/>
-      <c r="U20" s="58"/>
-      <c r="V20" s="58"/>
+      <c r="Q20" s="57"/>
+      <c r="R20" s="57"/>
+      <c r="S20" s="57"/>
+      <c r="T20" s="57"/>
+      <c r="U20" s="57"/>
+      <c r="V20" s="57"/>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B21" s="65" t="s">
+      <c r="B21" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="64" t="s">
         <v>123</v>
       </c>
-      <c r="C21" s="65" t="s">
-        <v>125</v>
-      </c>
-      <c r="D21" s="65" t="s">
-        <v>131</v>
-      </c>
-      <c r="E21" s="65" t="s">
+      <c r="D21" s="64" t="s">
+        <v>129</v>
+      </c>
+      <c r="E21" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" s="16" t="s">
         <v>124</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>126</v>
       </c>
       <c r="G21" s="21"/>
       <c r="H21" s="21"/>
       <c r="I21" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="K21" s="65" t="s">
-        <v>131</v>
-      </c>
-      <c r="L21" s="65" t="s">
-        <v>125</v>
-      </c>
-      <c r="M21" s="65" t="s">
+        <v>122</v>
+      </c>
+      <c r="K21" s="64" t="s">
+        <v>129</v>
+      </c>
+      <c r="L21" s="64" t="s">
         <v>123</v>
       </c>
-      <c r="Q21" s="58"/>
-      <c r="R21" s="58"/>
-      <c r="S21" s="58"/>
-      <c r="T21" s="58"/>
-      <c r="U21" s="58"/>
-      <c r="V21" s="58"/>
-      <c r="AA21" s="58"/>
+      <c r="M21" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q21" s="57"/>
+      <c r="R21" s="57"/>
+      <c r="S21" s="57"/>
+      <c r="T21" s="57"/>
+      <c r="U21" s="57"/>
+      <c r="V21" s="57"/>
+      <c r="AA21" s="57"/>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B22" s="66" t="s">
-        <v>152</v>
-      </c>
-      <c r="C22" s="78" t="s">
-        <v>163</v>
-      </c>
-      <c r="D22" s="77"/>
-      <c r="E22" s="61" t="s">
-        <v>184</v>
+      <c r="B22" s="65" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" s="77" t="s">
+        <v>159</v>
+      </c>
+      <c r="D22" s="76"/>
+      <c r="E22" s="60" t="s">
+        <v>180</v>
       </c>
       <c r="F22" s="6">
         <v>1</v>
@@ -2282,35 +2266,35 @@
       <c r="J22" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="K22" s="71" t="s">
+      <c r="K22" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="L22" s="58" t="s">
+        <v>157</v>
+      </c>
+      <c r="M22" s="65" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q22" s="57"/>
+      <c r="R22" s="57"/>
+      <c r="S22" s="57"/>
+      <c r="T22" s="57"/>
+      <c r="U22" s="57"/>
+      <c r="V22" s="57"/>
+      <c r="AA22" s="57"/>
+    </row>
+    <row r="23" spans="2:27" x14ac:dyDescent="0.15">
+      <c r="B23" s="65" t="s">
+        <v>163</v>
+      </c>
+      <c r="C23" s="66" t="s">
         <v>162</v>
       </c>
-      <c r="L22" s="59" t="s">
+      <c r="D23" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="E23" s="59" t="s">
         <v>161</v>
-      </c>
-      <c r="M22" s="66" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q22" s="58"/>
-      <c r="R22" s="58"/>
-      <c r="S22" s="58"/>
-      <c r="T22" s="58"/>
-      <c r="U22" s="58"/>
-      <c r="V22" s="58"/>
-      <c r="AA22" s="58"/>
-    </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B23" s="66" t="s">
-        <v>167</v>
-      </c>
-      <c r="C23" s="67" t="s">
-        <v>166</v>
-      </c>
-      <c r="D23" s="71" t="s">
-        <v>162</v>
-      </c>
-      <c r="E23" s="60" t="s">
-        <v>165</v>
       </c>
       <c r="F23" s="6">
         <v>2</v>
@@ -2323,35 +2307,35 @@
       <c r="J23" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K23" s="71" t="s">
-        <v>162</v>
-      </c>
-      <c r="L23" s="59" t="s">
+      <c r="K23" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="L23" s="58" t="s">
+        <v>160</v>
+      </c>
+      <c r="M23" s="65" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q23" s="57"/>
+      <c r="R23" s="57"/>
+      <c r="S23" s="57"/>
+      <c r="T23" s="57"/>
+      <c r="U23" s="57"/>
+      <c r="V23" s="57"/>
+      <c r="AA23" s="57"/>
+    </row>
+    <row r="24" spans="2:27" x14ac:dyDescent="0.15">
+      <c r="B24" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="C24" s="66" t="s">
+        <v>166</v>
+      </c>
+      <c r="D24" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="E24" s="60" t="s">
         <v>164</v>
-      </c>
-      <c r="M23" s="66" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q23" s="58"/>
-      <c r="R23" s="58"/>
-      <c r="S23" s="58"/>
-      <c r="T23" s="58"/>
-      <c r="U23" s="58"/>
-      <c r="V23" s="58"/>
-      <c r="AA23" s="58"/>
-    </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B24" s="61" t="s">
-        <v>170</v>
-      </c>
-      <c r="C24" s="67" t="s">
-        <v>170</v>
-      </c>
-      <c r="D24" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="E24" s="61" t="s">
-        <v>168</v>
       </c>
       <c r="F24" s="6">
         <v>3</v>
@@ -2364,34 +2348,34 @@
       <c r="J24" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K24" s="71" t="s">
-        <v>182</v>
-      </c>
-      <c r="L24" s="59" t="s">
-        <v>155</v>
-      </c>
-      <c r="M24" s="66" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q24" s="58"/>
-      <c r="R24" s="58"/>
-      <c r="S24" s="58"/>
-      <c r="T24" s="58"/>
-      <c r="U24" s="58"/>
-      <c r="V24" s="58"/>
-      <c r="AA24" s="58"/>
+      <c r="K24" s="70" t="s">
+        <v>178</v>
+      </c>
+      <c r="L24" s="58" t="s">
+        <v>151</v>
+      </c>
+      <c r="M24" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q24" s="57"/>
+      <c r="R24" s="57"/>
+      <c r="S24" s="57"/>
+      <c r="T24" s="57"/>
+      <c r="U24" s="57"/>
+      <c r="V24" s="57"/>
+      <c r="AA24" s="57"/>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B25" s="61" t="s">
-        <v>171</v>
-      </c>
-      <c r="C25" s="67" t="s">
-        <v>171</v>
-      </c>
-      <c r="D25" s="75" t="s">
-        <v>169</v>
-      </c>
-      <c r="E25" s="60" t="s">
+      <c r="B25" s="60" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25" s="66" t="s">
+        <v>167</v>
+      </c>
+      <c r="D25" s="74" t="s">
+        <v>165</v>
+      </c>
+      <c r="E25" s="59" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="6">
@@ -2405,34 +2389,34 @@
       <c r="J25" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K25" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="L25" s="59" t="s">
-        <v>156</v>
-      </c>
-      <c r="M25" s="61" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q25" s="58"/>
-      <c r="R25" s="58"/>
-      <c r="S25" s="58"/>
-      <c r="T25" s="58"/>
-      <c r="U25" s="58"/>
-      <c r="V25" s="58"/>
-      <c r="AA25" s="58"/>
+      <c r="K25" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="L25" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="M25" s="60" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q25" s="57"/>
+      <c r="R25" s="57"/>
+      <c r="S25" s="57"/>
+      <c r="T25" s="57"/>
+      <c r="U25" s="57"/>
+      <c r="V25" s="57"/>
+      <c r="AA25" s="57"/>
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B26" s="61" t="s">
-        <v>172</v>
-      </c>
-      <c r="C26" s="67" t="s">
-        <v>172</v>
-      </c>
-      <c r="D26" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="E26" s="60" t="s">
+      <c r="B26" s="60" t="s">
+        <v>168</v>
+      </c>
+      <c r="C26" s="66" t="s">
+        <v>168</v>
+      </c>
+      <c r="D26" s="75" t="s">
+        <v>165</v>
+      </c>
+      <c r="E26" s="59" t="s">
         <v>9</v>
       </c>
       <c r="F26" s="6">
@@ -2446,34 +2430,34 @@
       <c r="J26" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K26" s="71" t="s">
+      <c r="K26" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="L26" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="M26" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q26" s="57"/>
+      <c r="R26" s="57"/>
+      <c r="S26" s="57"/>
+      <c r="T26" s="57"/>
+      <c r="U26" s="57"/>
+      <c r="V26" s="57"/>
+      <c r="AA26" s="57"/>
+    </row>
+    <row r="27" spans="2:27" x14ac:dyDescent="0.15">
+      <c r="B27" s="60" t="s">
         <v>169</v>
       </c>
-      <c r="L26" s="59" t="s">
-        <v>30</v>
-      </c>
-      <c r="M26" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q26" s="58"/>
-      <c r="R26" s="58"/>
-      <c r="S26" s="58"/>
-      <c r="T26" s="58"/>
-      <c r="U26" s="58"/>
-      <c r="V26" s="58"/>
-      <c r="AA26" s="58"/>
-    </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B27" s="61" t="s">
-        <v>173</v>
-      </c>
-      <c r="C27" s="67" t="s">
-        <v>173</v>
-      </c>
-      <c r="D27" s="71" t="s">
+      <c r="C27" s="66" t="s">
         <v>169</v>
       </c>
-      <c r="E27" s="62" t="s">
+      <c r="D27" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="E27" s="61" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="6">
@@ -2487,34 +2471,34 @@
       <c r="J27" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K27" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="L27" s="59" t="s">
-        <v>157</v>
-      </c>
-      <c r="M27" s="61" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q27" s="58"/>
-      <c r="R27" s="58"/>
-      <c r="S27" s="58"/>
-      <c r="T27" s="58"/>
-      <c r="U27" s="58"/>
-      <c r="V27" s="58"/>
-      <c r="AA27" s="58"/>
+      <c r="K27" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="L27" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="M27" s="60" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q27" s="57"/>
+      <c r="R27" s="57"/>
+      <c r="S27" s="57"/>
+      <c r="T27" s="57"/>
+      <c r="U27" s="57"/>
+      <c r="V27" s="57"/>
+      <c r="AA27" s="57"/>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B28" s="61" t="s">
-        <v>174</v>
-      </c>
-      <c r="C28" s="67" t="s">
-        <v>174</v>
-      </c>
-      <c r="D28" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="E28" s="62" t="s">
+      <c r="B28" s="60" t="s">
+        <v>170</v>
+      </c>
+      <c r="C28" s="66" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="E28" s="61" t="s">
         <v>13</v>
       </c>
       <c r="F28" s="7">
@@ -2528,33 +2512,33 @@
       <c r="J28" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K28" s="72"/>
-      <c r="L28" s="68" t="s">
-        <v>163</v>
-      </c>
-      <c r="M28" s="66" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q28" s="58"/>
-      <c r="R28" s="58"/>
-      <c r="S28" s="58"/>
-      <c r="T28" s="58"/>
-      <c r="U28" s="58"/>
-      <c r="V28" s="58"/>
-      <c r="AA28" s="58"/>
+      <c r="K28" s="71"/>
+      <c r="L28" s="67" t="s">
+        <v>159</v>
+      </c>
+      <c r="M28" s="65" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q28" s="57"/>
+      <c r="R28" s="57"/>
+      <c r="S28" s="57"/>
+      <c r="T28" s="57"/>
+      <c r="U28" s="57"/>
+      <c r="V28" s="57"/>
+      <c r="AA28" s="57"/>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B29" s="66" t="s">
-        <v>175</v>
-      </c>
-      <c r="C29" s="67" t="s">
-        <v>175</v>
-      </c>
-      <c r="D29" s="71" t="s">
-        <v>176</v>
-      </c>
-      <c r="E29" s="63" t="s">
-        <v>175</v>
+      <c r="B29" s="65" t="s">
+        <v>171</v>
+      </c>
+      <c r="C29" s="66" t="s">
+        <v>171</v>
+      </c>
+      <c r="D29" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="E29" s="62" t="s">
+        <v>171</v>
       </c>
       <c r="F29" s="7">
         <v>8</v>
@@ -2567,35 +2551,35 @@
       <c r="J29" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K29" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="L29" s="59" t="s">
-        <v>158</v>
-      </c>
-      <c r="M29" s="61" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q29" s="58"/>
-      <c r="R29" s="58"/>
-      <c r="S29" s="58"/>
-      <c r="T29" s="58"/>
-      <c r="U29" s="58"/>
-      <c r="V29" s="58"/>
-      <c r="AA29" s="58"/>
+      <c r="K29" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="L29" s="58" t="s">
+        <v>154</v>
+      </c>
+      <c r="M29" s="60" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q29" s="57"/>
+      <c r="R29" s="57"/>
+      <c r="S29" s="57"/>
+      <c r="T29" s="57"/>
+      <c r="U29" s="57"/>
+      <c r="V29" s="57"/>
+      <c r="AA29" s="57"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B30" s="66" t="s">
-        <v>177</v>
-      </c>
-      <c r="C30" s="67" t="s">
-        <v>177</v>
-      </c>
-      <c r="D30" s="71" t="s">
-        <v>178</v>
-      </c>
-      <c r="E30" s="63" t="s">
-        <v>177</v>
+      <c r="B30" s="65" t="s">
+        <v>173</v>
+      </c>
+      <c r="C30" s="66" t="s">
+        <v>173</v>
+      </c>
+      <c r="D30" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="E30" s="62" t="s">
+        <v>173</v>
       </c>
       <c r="F30" s="7">
         <v>9</v>
@@ -2608,35 +2592,35 @@
       <c r="J30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="K30" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="L30" s="59" t="s">
-        <v>159</v>
-      </c>
-      <c r="M30" s="61" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q30" s="58"/>
-      <c r="R30" s="58"/>
-      <c r="S30" s="58"/>
-      <c r="T30" s="58"/>
-      <c r="U30" s="58"/>
-      <c r="V30" s="58"/>
-      <c r="AA30" s="61"/>
+      <c r="K30" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="L30" s="58" t="s">
+        <v>155</v>
+      </c>
+      <c r="M30" s="60" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q30" s="57"/>
+      <c r="R30" s="57"/>
+      <c r="S30" s="57"/>
+      <c r="T30" s="57"/>
+      <c r="U30" s="57"/>
+      <c r="V30" s="57"/>
+      <c r="AA30" s="60"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B31" s="61" t="s">
-        <v>180</v>
-      </c>
-      <c r="C31" s="70" t="s">
-        <v>180</v>
-      </c>
-      <c r="D31" s="74" t="s">
-        <v>169</v>
-      </c>
-      <c r="E31" s="64" t="s">
-        <v>179</v>
+      <c r="B31" s="60" t="s">
+        <v>176</v>
+      </c>
+      <c r="C31" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="D31" s="73" t="s">
+        <v>165</v>
+      </c>
+      <c r="E31" s="63" t="s">
+        <v>175</v>
       </c>
       <c r="F31" s="14">
         <v>10</v>
@@ -2649,32 +2633,32 @@
       <c r="J31" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="K31" s="73"/>
-      <c r="L31" s="69" t="s">
-        <v>160</v>
-      </c>
-      <c r="M31" s="66" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q31" s="58"/>
-      <c r="R31" s="58"/>
-      <c r="S31" s="58"/>
-      <c r="T31" s="58"/>
-      <c r="U31" s="58"/>
-      <c r="V31" s="58"/>
-      <c r="AA31" s="58"/>
+      <c r="K31" s="72"/>
+      <c r="L31" s="68" t="s">
+        <v>156</v>
+      </c>
+      <c r="M31" s="65" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q31" s="57"/>
+      <c r="R31" s="57"/>
+      <c r="S31" s="57"/>
+      <c r="T31" s="57"/>
+      <c r="U31" s="57"/>
+      <c r="V31" s="57"/>
+      <c r="AA31" s="57"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.15">
       <c r="E32"/>
-      <c r="Q32" s="58"/>
-      <c r="R32" s="58"/>
-      <c r="S32" s="58"/>
-      <c r="T32" s="58"/>
-      <c r="U32" s="58"/>
-      <c r="V32" s="58"/>
+      <c r="Q32" s="57"/>
+      <c r="R32" s="57"/>
+      <c r="S32" s="57"/>
+      <c r="T32" s="57"/>
+      <c r="U32" s="57"/>
+      <c r="V32" s="57"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B34" s="38"/>
+      <c r="B34" s="37"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -2687,271 +2671,271 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="20"/>
-      <c r="O34" s="40"/>
+      <c r="O34" s="39"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B35" s="37"/>
-      <c r="C35" s="41" t="s">
-        <v>144</v>
-      </c>
-      <c r="D35" s="42"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="40" t="s">
+        <v>141</v>
+      </c>
+      <c r="D35" s="41"/>
       <c r="E35" t="s">
-        <v>143</v>
-      </c>
-      <c r="K35" s="42"/>
+        <v>140</v>
+      </c>
+      <c r="K35" s="41"/>
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
       <c r="N35" s="9"/>
-      <c r="O35" s="43"/>
+      <c r="O35" s="42"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B36" s="37"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="42"/>
-      <c r="K36" s="42"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="41"/>
+      <c r="K36" s="41"/>
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
       <c r="N36" s="9"/>
-      <c r="O36" s="43"/>
+      <c r="O36" s="42"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B37" s="37"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="42"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="41"/>
       <c r="E37" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
       <c r="I37" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J37" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="K37" s="42"/>
+        <v>121</v>
+      </c>
+      <c r="K37" s="41"/>
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
       <c r="N37" s="9"/>
-      <c r="O37" s="43"/>
+      <c r="O37" s="42"/>
     </row>
     <row r="38" spans="2:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B38" s="37"/>
+      <c r="B38" s="36"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="9"/>
-      <c r="G38" s="83">
+      <c r="G38" s="82">
         <v>8</v>
       </c>
-      <c r="H38" s="84"/>
+      <c r="H38" s="83"/>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
       <c r="N38" s="9"/>
-      <c r="O38" s="43"/>
+      <c r="O38" s="42"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B39" s="37"/>
+      <c r="B39" s="36"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F39" s="8">
         <v>1</v>
       </c>
-      <c r="G39" s="79"/>
-      <c r="H39" s="80"/>
-      <c r="I39" s="45">
+      <c r="G39" s="78"/>
+      <c r="H39" s="79"/>
+      <c r="I39" s="44">
         <v>16</v>
       </c>
       <c r="J39" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
       <c r="N39" s="9"/>
-      <c r="O39" s="43"/>
+      <c r="O39" s="42"/>
     </row>
     <row r="40" spans="2:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B40" s="37"/>
+      <c r="B40" s="36"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F40" s="8">
         <v>2</v>
       </c>
-      <c r="G40" s="79">
+      <c r="G40" s="78">
         <v>8</v>
       </c>
-      <c r="H40" s="80"/>
-      <c r="I40" s="45">
+      <c r="H40" s="79"/>
+      <c r="I40" s="44">
         <v>15</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
       <c r="M40" s="8"/>
       <c r="N40" s="9"/>
-      <c r="O40" s="43"/>
+      <c r="O40" s="42"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B41" s="37"/>
+      <c r="B41" s="36"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F41" s="8">
         <v>3</v>
       </c>
-      <c r="G41" s="79"/>
-      <c r="H41" s="80"/>
-      <c r="I41" s="45">
+      <c r="G41" s="78"/>
+      <c r="H41" s="79"/>
+      <c r="I41" s="44">
         <v>14</v>
       </c>
       <c r="J41" s="9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="K41" s="8"/>
       <c r="L41" s="8"/>
       <c r="M41" s="8"/>
       <c r="N41" s="9"/>
-      <c r="O41" s="43"/>
+      <c r="O41" s="42"/>
     </row>
     <row r="42" spans="2:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B42" s="37"/>
+      <c r="B42" s="36"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8" t="s">
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="F42" s="8">
         <v>4</v>
       </c>
-      <c r="G42" s="79" t="s">
-        <v>37</v>
-      </c>
-      <c r="H42" s="80"/>
-      <c r="I42" s="45">
+      <c r="G42" s="78" t="s">
+        <v>36</v>
+      </c>
+      <c r="H42" s="79"/>
+      <c r="I42" s="44">
         <v>13</v>
       </c>
-      <c r="J42" s="45" t="s">
-        <v>138</v>
+      <c r="J42" s="44" t="s">
+        <v>135</v>
       </c>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
       <c r="M42" s="8"/>
       <c r="N42" s="9"/>
-      <c r="O42" s="43"/>
+      <c r="O42" s="42"/>
     </row>
     <row r="43" spans="2:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B43" s="37"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F43" s="8">
         <v>5</v>
       </c>
-      <c r="G43" s="79">
+      <c r="G43" s="78">
         <v>8</v>
       </c>
-      <c r="H43" s="80"/>
-      <c r="I43" s="45">
+      <c r="H43" s="79"/>
+      <c r="I43" s="44">
         <v>12</v>
       </c>
-      <c r="J43" s="45" t="s">
-        <v>181</v>
+      <c r="J43" s="44" t="s">
+        <v>177</v>
       </c>
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
       <c r="M43" s="8"/>
       <c r="N43" s="9"/>
-      <c r="O43" s="43"/>
+      <c r="O43" s="42"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B44" s="37"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F44" s="8">
         <v>6</v>
       </c>
-      <c r="G44" s="79"/>
-      <c r="H44" s="80"/>
-      <c r="I44" s="45">
+      <c r="G44" s="78"/>
+      <c r="H44" s="79"/>
+      <c r="I44" s="44">
         <v>11</v>
       </c>
-      <c r="J44" s="45" t="s">
-        <v>141</v>
+      <c r="J44" s="44" t="s">
+        <v>138</v>
       </c>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
       <c r="M44" s="8"/>
       <c r="N44" s="9"/>
-      <c r="O44" s="43"/>
+      <c r="O44" s="42"/>
     </row>
     <row r="45" spans="2:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B45" s="37"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
       <c r="F45" s="10">
         <v>7</v>
       </c>
-      <c r="G45" s="79">
+      <c r="G45" s="78">
         <v>8</v>
       </c>
-      <c r="H45" s="80"/>
-      <c r="I45" s="45">
+      <c r="H45" s="79"/>
+      <c r="I45" s="44">
         <v>10</v>
       </c>
-      <c r="J45" s="45"/>
+      <c r="J45" s="44"/>
       <c r="K45" s="8"/>
       <c r="L45" s="8"/>
       <c r="M45" s="8"/>
       <c r="N45" s="9"/>
-      <c r="O45" s="43"/>
+      <c r="O45" s="42"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B46" s="37"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F46" s="10">
         <v>8</v>
       </c>
-      <c r="G46" s="81"/>
-      <c r="H46" s="82"/>
-      <c r="I46" s="45">
+      <c r="G46" s="80"/>
+      <c r="H46" s="81"/>
+      <c r="I46" s="44">
         <v>9</v>
       </c>
-      <c r="J46" s="45"/>
+      <c r="J46" s="44"/>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
       <c r="M46" s="8"/>
       <c r="N46" s="9"/>
-      <c r="O46" s="43"/>
+      <c r="O46" s="42"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B47" s="37"/>
+      <c r="B47" s="36"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
@@ -2964,10 +2948,10 @@
       <c r="L47" s="8"/>
       <c r="M47" s="8"/>
       <c r="N47" s="9"/>
-      <c r="O47" s="43"/>
+      <c r="O47" s="42"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B48" s="37"/>
+      <c r="B48" s="36"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
@@ -2980,10 +2964,10 @@
       <c r="L48" s="8"/>
       <c r="M48" s="8"/>
       <c r="N48" s="9"/>
-      <c r="O48" s="43"/>
+      <c r="O48" s="42"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B49" s="37"/>
+      <c r="B49" s="36"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
@@ -2996,10 +2980,10 @@
       <c r="L49" s="8"/>
       <c r="M49" s="8"/>
       <c r="N49" s="9"/>
-      <c r="O49" s="43"/>
+      <c r="O49" s="42"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B50" s="37"/>
+      <c r="B50" s="36"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
@@ -3012,10 +2996,10 @@
       <c r="L50" s="8"/>
       <c r="M50" s="8"/>
       <c r="N50" s="9"/>
-      <c r="O50" s="43"/>
+      <c r="O50" s="42"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B51" s="37"/>
+      <c r="B51" s="36"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
@@ -3028,10 +3012,10 @@
       <c r="L51" s="8"/>
       <c r="M51" s="8"/>
       <c r="N51" s="9"/>
-      <c r="O51" s="43"/>
+      <c r="O51" s="42"/>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B52" s="37"/>
+      <c r="B52" s="36"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
@@ -3044,10 +3028,10 @@
       <c r="L52" s="8"/>
       <c r="M52" s="8"/>
       <c r="N52" s="9"/>
-      <c r="O52" s="43"/>
+      <c r="O52" s="42"/>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B53" s="37"/>
+      <c r="B53" s="36"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
@@ -3060,10 +3044,10 @@
       <c r="L53" s="8"/>
       <c r="M53" s="8"/>
       <c r="N53" s="9"/>
-      <c r="O53" s="43"/>
+      <c r="O53" s="42"/>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B54" s="37"/>
+      <c r="B54" s="36"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
@@ -3076,10 +3060,10 @@
       <c r="L54" s="8"/>
       <c r="M54" s="8"/>
       <c r="N54" s="9"/>
-      <c r="O54" s="43"/>
+      <c r="O54" s="42"/>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B55" s="37"/>
+      <c r="B55" s="36"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
@@ -3092,10 +3076,10 @@
       <c r="L55" s="8"/>
       <c r="M55" s="8"/>
       <c r="N55" s="9"/>
-      <c r="O55" s="43"/>
+      <c r="O55" s="42"/>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B56" s="37"/>
+      <c r="B56" s="36"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
@@ -3108,11 +3092,11 @@
       <c r="L56" s="8"/>
       <c r="M56" s="8"/>
       <c r="N56" s="9"/>
-      <c r="O56" s="43"/>
+      <c r="O56" s="42"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B57" s="37"/>
-      <c r="C57" s="42"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="41"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
       <c r="F57" s="9"/>
@@ -3124,11 +3108,11 @@
       <c r="L57" s="8"/>
       <c r="M57" s="8"/>
       <c r="N57" s="9"/>
-      <c r="O57" s="43"/>
+      <c r="O57" s="42"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B58" s="37"/>
-      <c r="C58" s="42"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="41"/>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
       <c r="F58" s="9"/>
@@ -3140,11 +3124,11 @@
       <c r="L58" s="8"/>
       <c r="M58" s="8"/>
       <c r="N58" s="9"/>
-      <c r="O58" s="43"/>
+      <c r="O58" s="42"/>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B59" s="37"/>
-      <c r="C59" s="42"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="41"/>
       <c r="D59" s="8"/>
       <c r="E59" s="8"/>
       <c r="F59" s="9"/>
@@ -3156,10 +3140,10 @@
       <c r="L59" s="8"/>
       <c r="M59" s="8"/>
       <c r="N59" s="9"/>
-      <c r="O59" s="43"/>
+      <c r="O59" s="42"/>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B60" s="35"/>
+      <c r="B60" s="34"/>
       <c r="C60" s="16"/>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
@@ -3172,7 +3156,7 @@
       <c r="L60" s="16"/>
       <c r="M60" s="16"/>
       <c r="N60" s="21"/>
-      <c r="O60" s="36"/>
+      <c r="O60" s="35"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L5:M9">
@@ -3221,73 +3205,73 @@
   <sheetData>
     <row r="2" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="X2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AC2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="2:31" x14ac:dyDescent="0.15">
       <c r="R3" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="S3" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="T3" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="S3" s="17" t="s">
+      <c r="U3" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="T3" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="U3" s="17" t="s">
-        <v>75</v>
       </c>
       <c r="W3" s="27"/>
       <c r="X3" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Y3" s="25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="Z3" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AB3" s="27"/>
       <c r="AC3" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AD3" s="25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AE3" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="2:31" x14ac:dyDescent="0.15">
       <c r="H4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" t="s">
         <v>64</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>65</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>66</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>67</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>68</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>69</v>
-      </c>
-      <c r="N4" t="s">
-        <v>70</v>
-      </c>
-      <c r="O4" t="s">
-        <v>71</v>
       </c>
       <c r="R4" s="17">
         <v>8</v>
@@ -3302,28 +3286,28 @@
         <v>1</v>
       </c>
       <c r="W4" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="X4" s="20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Y4" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="Z4" s="32" t="s">
-        <v>90</v>
+        <v>116</v>
+      </c>
+      <c r="Z4" s="31" t="s">
+        <v>88</v>
       </c>
       <c r="AB4" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AC4" s="20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AD4" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="AE4" s="32" t="s">
-        <v>90</v>
+        <v>112</v>
+      </c>
+      <c r="AE4" s="31" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="2:31" ht="5.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3333,11 +3317,11 @@
       <c r="W5" s="29"/>
       <c r="X5" s="9"/>
       <c r="Y5" s="23"/>
-      <c r="Z5" s="33"/>
+      <c r="Z5" s="32"/>
       <c r="AB5" s="29"/>
       <c r="AC5" s="9"/>
       <c r="AD5" s="23"/>
-      <c r="AE5" s="33"/>
+      <c r="AE5" s="32"/>
     </row>
     <row r="6" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B6">
@@ -3394,24 +3378,24 @@
         <v>0</v>
       </c>
       <c r="W6" s="29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="X6" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Y6" s="23"/>
-      <c r="Z6" s="33" t="s">
-        <v>92</v>
+      <c r="Z6" s="32" t="s">
+        <v>90</v>
       </c>
       <c r="AB6" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AC6" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AD6" s="23"/>
-      <c r="AE6" s="33" t="s">
-        <v>91</v>
+      <c r="AE6" s="32" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="2:31" ht="4.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3419,11 +3403,11 @@
       <c r="W7" s="29"/>
       <c r="X7" s="9"/>
       <c r="Y7" s="23"/>
-      <c r="Z7" s="33"/>
+      <c r="Z7" s="32"/>
       <c r="AB7" s="29"/>
       <c r="AC7" s="9"/>
       <c r="AD7" s="23"/>
-      <c r="AE7" s="33"/>
+      <c r="AE7" s="32"/>
     </row>
     <row r="8" spans="2:31" x14ac:dyDescent="0.15">
       <c r="C8" s="19">
@@ -3433,24 +3417,24 @@
         <v>1</v>
       </c>
       <c r="W8" s="29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="X8" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Y8" s="23"/>
-      <c r="Z8" s="33" t="s">
-        <v>92</v>
+      <c r="Z8" s="32" t="s">
+        <v>90</v>
       </c>
       <c r="AB8" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AC8" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AD8" s="23"/>
-      <c r="AE8" s="33" t="s">
-        <v>91</v>
+      <c r="AE8" s="32" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="2:31" ht="5.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3461,36 +3445,36 @@
       <c r="W9" s="29"/>
       <c r="X9" s="9"/>
       <c r="Y9" s="23"/>
-      <c r="Z9" s="33"/>
+      <c r="Z9" s="32"/>
       <c r="AB9" s="29"/>
       <c r="AC9" s="9"/>
       <c r="AD9" s="23"/>
-      <c r="AE9" s="33"/>
+      <c r="AE9" s="32"/>
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.15">
       <c r="W10" s="29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="X10" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Y10" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="Z10" s="33" t="s">
-        <v>90</v>
+        <v>83</v>
+      </c>
+      <c r="Z10" s="32" t="s">
+        <v>88</v>
       </c>
       <c r="AB10" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC10" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AD10" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="AE10" s="33" t="s">
-        <v>90</v>
+        <v>113</v>
+      </c>
+      <c r="AE10" s="32" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="2:31" ht="5.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3498,11 +3482,11 @@
       <c r="W11" s="29"/>
       <c r="X11" s="9"/>
       <c r="Y11" s="23"/>
-      <c r="Z11" s="33"/>
+      <c r="Z11" s="32"/>
       <c r="AB11" s="29"/>
       <c r="AC11" s="9"/>
       <c r="AD11" s="23"/>
-      <c r="AE11" s="33"/>
+      <c r="AE11" s="32"/>
     </row>
     <row r="12" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B12">
@@ -3557,24 +3541,24 @@
         <v>1</v>
       </c>
       <c r="W12" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X12" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Y12" s="23"/>
-      <c r="Z12" s="33" t="s">
-        <v>91</v>
+      <c r="Z12" s="32" t="s">
+        <v>89</v>
       </c>
       <c r="AB12" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AC12" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AD12" s="23"/>
-      <c r="AE12" s="33" t="s">
-        <v>91</v>
+      <c r="AE12" s="32" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="2:31" ht="4.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3582,11 +3566,11 @@
       <c r="W13" s="29"/>
       <c r="X13" s="9"/>
       <c r="Y13" s="23"/>
-      <c r="Z13" s="33"/>
+      <c r="Z13" s="32"/>
       <c r="AB13" s="29"/>
       <c r="AC13" s="9"/>
       <c r="AD13" s="23"/>
-      <c r="AE13" s="33"/>
+      <c r="AE13" s="32"/>
     </row>
     <row r="14" spans="2:31" x14ac:dyDescent="0.15">
       <c r="C14" s="19"/>
@@ -3594,28 +3578,28 @@
         <v>1</v>
       </c>
       <c r="W14" s="29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="X14" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Y14" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z14" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="Z14" s="33" t="s">
-        <v>91</v>
-      </c>
       <c r="AB14" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC14" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="AD14" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE14" s="33" t="s">
-        <v>91</v>
+        <v>114</v>
+      </c>
+      <c r="AE14" s="32" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="2:31" ht="5.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3624,36 +3608,36 @@
       <c r="W15" s="29"/>
       <c r="X15" s="9"/>
       <c r="Y15" s="23"/>
-      <c r="Z15" s="33"/>
+      <c r="Z15" s="32"/>
       <c r="AB15" s="29"/>
       <c r="AC15" s="9"/>
       <c r="AD15" s="23"/>
-      <c r="AE15" s="33"/>
+      <c r="AE15" s="32"/>
     </row>
     <row r="16" spans="2:31" x14ac:dyDescent="0.15">
       <c r="W16" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="X16" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Y16" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z16" s="33" t="s">
-        <v>90</v>
+        <v>84</v>
+      </c>
+      <c r="Z16" s="32" t="s">
+        <v>88</v>
       </c>
       <c r="AB16" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AC16" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AD16" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="AE16" s="33" t="s">
-        <v>90</v>
+        <v>115</v>
+      </c>
+      <c r="AE16" s="32" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="2:31" ht="5.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3663,11 +3647,11 @@
       <c r="W17" s="30"/>
       <c r="X17" s="21"/>
       <c r="Y17" s="24"/>
-      <c r="Z17" s="34"/>
+      <c r="Z17" s="33"/>
       <c r="AB17" s="30"/>
       <c r="AC17" s="21"/>
       <c r="AD17" s="24"/>
-      <c r="AE17" s="34"/>
+      <c r="AE17" s="33"/>
     </row>
     <row r="18" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B18">
@@ -3722,24 +3706,24 @@
         <v>0</v>
       </c>
       <c r="W18" s="29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="X18" s="9"/>
       <c r="Y18" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z18" s="33" t="s">
-        <v>92</v>
+        <v>99</v>
+      </c>
+      <c r="Z18" s="32" t="s">
+        <v>90</v>
       </c>
       <c r="AB18" s="29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AC18" s="9"/>
       <c r="AD18" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="AE18" s="33" t="s">
-        <v>91</v>
+        <v>99</v>
+      </c>
+      <c r="AE18" s="32" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="2:31" ht="4.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3749,11 +3733,11 @@
       <c r="W19" s="29"/>
       <c r="X19" s="9"/>
       <c r="Y19" s="23"/>
-      <c r="Z19" s="33"/>
+      <c r="Z19" s="32"/>
       <c r="AB19" s="29"/>
       <c r="AC19" s="9"/>
       <c r="AD19" s="23"/>
-      <c r="AE19" s="33"/>
+      <c r="AE19" s="32"/>
     </row>
     <row r="20" spans="2:31" x14ac:dyDescent="0.15">
       <c r="C20" s="19">
@@ -3761,24 +3745,24 @@
       </c>
       <c r="E20" s="19"/>
       <c r="W20" s="29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="X20" s="9"/>
       <c r="Y20" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z20" s="33" t="s">
-        <v>92</v>
+        <v>82</v>
+      </c>
+      <c r="Z20" s="32" t="s">
+        <v>90</v>
       </c>
       <c r="AB20" s="29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AC20" s="9"/>
       <c r="AD20" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="AE20" s="33" t="s">
-        <v>91</v>
+        <v>82</v>
+      </c>
+      <c r="AE20" s="32" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="2:31" ht="5.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3789,32 +3773,32 @@
       <c r="W21" s="29"/>
       <c r="X21" s="9"/>
       <c r="Y21" s="23"/>
-      <c r="Z21" s="33"/>
+      <c r="Z21" s="32"/>
       <c r="AB21" s="29"/>
       <c r="AC21" s="9"/>
       <c r="AD21" s="23"/>
-      <c r="AE21" s="33"/>
+      <c r="AE21" s="32"/>
     </row>
     <row r="22" spans="2:31" x14ac:dyDescent="0.15">
       <c r="W22" s="29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="X22" s="9"/>
       <c r="Y22" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z22" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="Z22" s="33" t="s">
-        <v>90</v>
-      </c>
       <c r="AB22" s="29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="AC22" s="9"/>
       <c r="AD22" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE22" s="32" t="s">
         <v>88</v>
-      </c>
-      <c r="AE22" s="33" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="23" spans="2:31" ht="5.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3824,11 +3808,11 @@
       <c r="W23" s="29"/>
       <c r="X23" s="9"/>
       <c r="Y23" s="23"/>
-      <c r="Z23" s="33"/>
+      <c r="Z23" s="32"/>
       <c r="AB23" s="29"/>
       <c r="AC23" s="9"/>
       <c r="AD23" s="23"/>
-      <c r="AE23" s="33"/>
+      <c r="AE23" s="32"/>
     </row>
     <row r="24" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B24">
@@ -3883,24 +3867,24 @@
         <v>1</v>
       </c>
       <c r="W24" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="X24" s="9"/>
       <c r="Y24" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z24" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z24" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB24" s="29" t="s">
         <v>92</v>
-      </c>
-      <c r="AB24" s="29" t="s">
-        <v>94</v>
       </c>
       <c r="AC24" s="9"/>
       <c r="AD24" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="AE24" s="33" t="s">
-        <v>91</v>
+        <v>93</v>
+      </c>
+      <c r="AE24" s="32" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="2:31" ht="4.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3910,34 +3894,34 @@
       <c r="W25" s="30"/>
       <c r="X25" s="21"/>
       <c r="Y25" s="24"/>
-      <c r="Z25" s="34"/>
+      <c r="Z25" s="33"/>
       <c r="AB25" s="30"/>
       <c r="AC25" s="21"/>
       <c r="AD25" s="24"/>
-      <c r="AE25" s="34"/>
+      <c r="AE25" s="33"/>
     </row>
     <row r="26" spans="2:31" x14ac:dyDescent="0.15">
       <c r="C26" s="19"/>
       <c r="E26" s="19">
         <v>1</v>
       </c>
-      <c r="W26" s="38"/>
+      <c r="W26" s="37"/>
       <c r="X26" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="Y26" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Z26" s="28">
         <v>4</v>
       </c>
       <c r="AA26" s="9"/>
-      <c r="AB26" s="38"/>
+      <c r="AB26" s="37"/>
       <c r="AC26" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="AD26" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AE26" s="28">
         <v>4</v>
@@ -3948,30 +3932,30 @@
         <v>1</v>
       </c>
       <c r="F27" s="19"/>
-      <c r="W27" s="37"/>
+      <c r="W27" s="36"/>
       <c r="X27" s="9"/>
-      <c r="Y27" s="39"/>
+      <c r="Y27" s="38"/>
       <c r="Z27" s="29"/>
       <c r="AA27" s="9"/>
-      <c r="AB27" s="37"/>
+      <c r="AB27" s="36"/>
       <c r="AC27" s="9"/>
-      <c r="AD27" s="39"/>
+      <c r="AD27" s="38"/>
       <c r="AE27" s="29"/>
     </row>
     <row r="28" spans="2:31" x14ac:dyDescent="0.15">
-      <c r="W28" s="35"/>
+      <c r="W28" s="34"/>
       <c r="X28" s="21"/>
       <c r="Y28" s="24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="Z28" s="30">
         <v>7</v>
       </c>
       <c r="AA28" s="9"/>
-      <c r="AB28" s="35"/>
+      <c r="AB28" s="34"/>
       <c r="AC28" s="21"/>
       <c r="AD28" s="24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AE28" s="30">
         <v>7</v>
@@ -4034,8 +4018,8 @@
       <c r="U30" s="17">
         <v>0</v>
       </c>
-      <c r="AC30" s="41" t="s">
-        <v>135</v>
+      <c r="AC30" s="40" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="2:31" ht="4.5" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>